<commit_message>
Update sense value spreadsheet to reflect changes made due to DAC selection
</commit_message>
<xml_diff>
--- a/sense_calculations.xlsx
+++ b/sense_calculations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikomo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\NikLoad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Sense resistor (R)</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Bandwidth/gain</t>
+  </si>
+  <si>
+    <t>Max - offset</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,17 +462,17 @@
       </c>
       <c r="C2">
         <f>(B2*$R$2)+$R$3</f>
-        <v>0.10002000000000001</v>
+        <v>0.10008</v>
       </c>
       <c r="D2">
-        <f>(A2^2)*$R$1</f>
+        <f t="shared" ref="D2:D33" si="0">(A2^2)*$R$1</f>
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="Q2" t="s">
         <v>1</v>
       </c>
       <c r="R2">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -477,15 +480,15 @@
         <v>0.01</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B54" si="0">A3*$R$1</f>
+        <f t="shared" ref="B3:B54" si="1">A3*$R$1</f>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C54" si="1">(B3*$R$2)+$R$3</f>
-        <v>0.10020000000000001</v>
+        <f t="shared" ref="C3:C54" si="2">(B3*$R$2)+$R$3</f>
+        <v>0.1008</v>
       </c>
       <c r="D3">
-        <f>(A3^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="Q3" t="s">
@@ -500,15 +503,15 @@
         <v>0.1</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>0.10200000000000001</v>
+        <f t="shared" si="2"/>
+        <v>0.10800000000000001</v>
       </c>
       <c r="D4">
-        <f>(A4^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>2.0000000000000005E-5</v>
       </c>
       <c r="Q4" t="s">
@@ -523,15 +526,15 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0.12000000000000001</v>
+        <f t="shared" si="2"/>
+        <v>0.18</v>
       </c>
       <c r="D5">
-        <f>(A5^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
       <c r="Q5" t="s">
@@ -539,7 +542,7 @@
       </c>
       <c r="R5" s="2">
         <f>R4/R2</f>
-        <v>1000000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -547,16 +550,23 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <f t="shared" si="2"/>
+        <v>0.26</v>
       </c>
       <c r="D6">
-        <f>(A6^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6">
+        <f>C54-R3</f>
+        <v>3.9999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -564,15 +574,15 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>0.16</v>
+        <f t="shared" si="2"/>
+        <v>0.33999999999999997</v>
       </c>
       <c r="D7">
-        <f>(A7^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="J7" s="3"/>
@@ -582,15 +592,15 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
+        <f t="shared" si="2"/>
+        <v>0.42000000000000004</v>
       </c>
       <c r="D8">
-        <f>(A8^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
@@ -599,15 +609,15 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.01</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
       <c r="D9">
-        <f>(A9^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
     </row>
@@ -616,15 +626,15 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2E-2</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>0.22</v>
+        <f t="shared" si="2"/>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D10">
-        <f>(A10^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>7.2000000000000008E-2</v>
       </c>
     </row>
@@ -633,15 +643,15 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4E-2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
-        <v>0.24000000000000002</v>
+        <f t="shared" si="2"/>
+        <v>0.66</v>
       </c>
       <c r="D11">
-        <f>(A11^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
@@ -650,15 +660,15 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
+        <f t="shared" si="2"/>
+        <v>0.74</v>
       </c>
       <c r="D12">
-        <f>(A12^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="J12" s="3"/>
@@ -668,15 +678,15 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
-        <v>0.28000000000000003</v>
+        <f t="shared" si="2"/>
+        <v>0.82000000000000006</v>
       </c>
       <c r="D13">
-        <f>(A13^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.16200000000000001</v>
       </c>
     </row>
@@ -685,15 +695,15 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="2"/>
+        <v>0.9</v>
       </c>
       <c r="D14">
-        <f>(A14^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -702,15 +712,15 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
-        <v>0.31999999999999995</v>
+        <f t="shared" si="2"/>
+        <v>0.97999999999999987</v>
       </c>
       <c r="D15">
-        <f>(A15^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.24199999999999999</v>
       </c>
     </row>
@@ -719,15 +729,15 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4E-2</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>0.33999999999999997</v>
+        <f t="shared" si="2"/>
+        <v>1.06</v>
       </c>
       <c r="D16">
-        <f>(A16^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.28800000000000003</v>
       </c>
       <c r="L16" s="3"/>
@@ -737,15 +747,15 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6000000000000002E-2</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
+        <f t="shared" si="2"/>
+        <v>1.1400000000000001</v>
       </c>
       <c r="D17">
-        <f>(A17^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.33800000000000002</v>
       </c>
     </row>
@@ -754,15 +764,15 @@
         <v>14</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
-        <v>0.38</v>
+        <f t="shared" si="2"/>
+        <v>1.2200000000000002</v>
       </c>
       <c r="D18">
-        <f>(A18^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.39200000000000002</v>
       </c>
     </row>
@@ -771,15 +781,15 @@
         <v>15</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f t="shared" si="2"/>
+        <v>1.3</v>
       </c>
       <c r="D19">
-        <f>(A19^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
     </row>
@@ -788,15 +798,15 @@
         <v>16</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
-        <v>0.42000000000000004</v>
+        <f t="shared" si="2"/>
+        <v>1.3800000000000001</v>
       </c>
       <c r="D20">
-        <f>(A20^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.51200000000000001</v>
       </c>
     </row>
@@ -805,15 +815,15 @@
         <v>17</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
-        <v>0.44000000000000006</v>
+        <f t="shared" si="2"/>
+        <v>1.4600000000000002</v>
       </c>
       <c r="D21">
-        <f>(A21^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.57799999999999996</v>
       </c>
     </row>
@@ -822,15 +832,15 @@
         <v>18</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
-        <v>0.46000000000000008</v>
+        <f t="shared" si="2"/>
+        <v>1.5400000000000003</v>
       </c>
       <c r="D22">
-        <f>(A22^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.64800000000000002</v>
       </c>
     </row>
@@ -839,15 +849,15 @@
         <v>19</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
+        <f t="shared" si="2"/>
+        <v>1.62</v>
       </c>
       <c r="D23">
-        <f>(A23^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.72199999999999998</v>
       </c>
     </row>
@@ -856,15 +866,15 @@
         <v>20</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>1.7000000000000002</v>
       </c>
       <c r="D24">
-        <f>(A24^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
@@ -873,15 +883,15 @@
         <v>21</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
-        <v>0.52</v>
+        <f t="shared" si="2"/>
+        <v>1.7800000000000002</v>
       </c>
       <c r="D25">
-        <f>(A25^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.88200000000000001</v>
       </c>
     </row>
@@ -890,15 +900,15 @@
         <v>22</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
-        <v>0.53999999999999992</v>
+        <f t="shared" si="2"/>
+        <v>1.8599999999999999</v>
       </c>
       <c r="D26">
-        <f>(A26^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>0.96799999999999997</v>
       </c>
     </row>
@@ -907,15 +917,15 @@
         <v>23</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
-        <v>0.55999999999999994</v>
+        <f t="shared" si="2"/>
+        <v>1.94</v>
       </c>
       <c r="D27">
-        <f>(A27^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.0580000000000001</v>
       </c>
     </row>
@@ -924,15 +934,15 @@
         <v>24</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
-        <v>0.57999999999999996</v>
+        <f t="shared" si="2"/>
+        <v>2.02</v>
       </c>
       <c r="D28">
-        <f>(A28^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.1520000000000001</v>
       </c>
     </row>
@@ -941,15 +951,15 @@
         <v>25</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f t="shared" si="2"/>
+        <v>2.1</v>
       </c>
       <c r="D29">
-        <f>(A29^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
@@ -958,15 +968,15 @@
         <v>26</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2000000000000005E-2</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
-        <v>0.62</v>
+        <f t="shared" si="2"/>
+        <v>2.1800000000000002</v>
       </c>
       <c r="D30">
-        <f>(A30^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.3520000000000001</v>
       </c>
     </row>
@@ -975,15 +985,15 @@
         <v>27</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
-        <v>0.64</v>
+        <f t="shared" si="2"/>
+        <v>2.2600000000000002</v>
       </c>
       <c r="D31">
-        <f>(A31^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.458</v>
       </c>
     </row>
@@ -992,15 +1002,15 @@
         <v>28</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
-        <v>0.66</v>
+        <f t="shared" si="2"/>
+        <v>2.3400000000000003</v>
       </c>
       <c r="D32">
-        <f>(A32^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.5680000000000001</v>
       </c>
     </row>
@@ -1009,15 +1019,15 @@
         <v>29</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
-        <v>0.68</v>
+        <f t="shared" si="2"/>
+        <v>2.4200000000000004</v>
       </c>
       <c r="D33">
-        <f>(A33^2)*$R$1</f>
+        <f t="shared" si="0"/>
         <v>1.6819999999999999</v>
       </c>
     </row>
@@ -1026,15 +1036,15 @@
         <v>30</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.06</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
-        <v>0.7</v>
+        <f t="shared" si="2"/>
+        <v>2.5</v>
       </c>
       <c r="D34">
-        <f>(A34^2)*$R$1</f>
+        <f t="shared" ref="D34:D54" si="3">(A34^2)*$R$1</f>
         <v>1.8</v>
       </c>
     </row>
@@ -1043,15 +1053,15 @@
         <v>31</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2E-2</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
+        <f t="shared" si="2"/>
+        <v>2.58</v>
       </c>
       <c r="D35">
-        <f>(A35^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>1.9219999999999999</v>
       </c>
     </row>
@@ -1060,15 +1070,15 @@
         <v>32</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
-        <v>0.74</v>
+        <f t="shared" si="2"/>
+        <v>2.66</v>
       </c>
       <c r="D36">
-        <f>(A36^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.048</v>
       </c>
     </row>
@@ -1077,15 +1087,15 @@
         <v>33</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
-        <v>0.76</v>
+        <f t="shared" si="2"/>
+        <v>2.74</v>
       </c>
       <c r="D37">
-        <f>(A37^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.1779999999999999</v>
       </c>
     </row>
@@ -1094,15 +1104,15 @@
         <v>34</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
-        <v>0.78</v>
+        <f t="shared" si="2"/>
+        <v>2.8200000000000003</v>
       </c>
       <c r="D38">
-        <f>(A38^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.3119999999999998</v>
       </c>
     </row>
@@ -1111,15 +1121,15 @@
         <v>35</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="2"/>
+        <v>2.9000000000000004</v>
       </c>
       <c r="D39">
-        <f>(A39^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.4500000000000002</v>
       </c>
     </row>
@@ -1128,15 +1138,15 @@
         <v>36</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.2000000000000008E-2</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
-        <v>0.82000000000000006</v>
+        <f t="shared" si="2"/>
+        <v>2.9800000000000004</v>
       </c>
       <c r="D40">
-        <f>(A40^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.5920000000000001</v>
       </c>
     </row>
@@ -1145,15 +1155,15 @@
         <v>37</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
-        <v>0.84</v>
+        <f t="shared" si="2"/>
+        <v>3.06</v>
       </c>
       <c r="D41">
-        <f>(A41^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.738</v>
       </c>
     </row>
@@ -1162,15 +1172,15 @@
         <v>38</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
-        <v>0.86</v>
+        <f t="shared" si="2"/>
+        <v>3.14</v>
       </c>
       <c r="D42">
-        <f>(A42^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>2.8879999999999999</v>
       </c>
     </row>
@@ -1179,15 +1189,15 @@
         <v>39</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8E-2</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
-        <v>0.88</v>
+        <f t="shared" si="2"/>
+        <v>3.22</v>
       </c>
       <c r="D43">
-        <f>(A43^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>3.0420000000000003</v>
       </c>
     </row>
@@ -1196,15 +1206,15 @@
         <v>40</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
-        <v>0.9</v>
+        <f t="shared" si="2"/>
+        <v>3.3000000000000003</v>
       </c>
       <c r="D44">
-        <f>(A44^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>3.2</v>
       </c>
     </row>
@@ -1213,15 +1223,15 @@
         <v>41</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
-        <v>0.92</v>
+        <f t="shared" si="2"/>
+        <v>3.3800000000000003</v>
       </c>
       <c r="D45">
-        <f>(A45^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>3.3620000000000001</v>
       </c>
     </row>
@@ -1230,15 +1240,15 @@
         <v>42</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
-        <v>0.94000000000000006</v>
+        <f t="shared" si="2"/>
+        <v>3.4600000000000004</v>
       </c>
       <c r="D46">
-        <f>(A46^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>3.528</v>
       </c>
     </row>
@@ -1247,15 +1257,15 @@
         <v>43</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6000000000000007E-2</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
-        <v>0.96000000000000008</v>
+        <f t="shared" si="2"/>
+        <v>3.5400000000000005</v>
       </c>
       <c r="D47">
-        <f>(A47^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>3.698</v>
       </c>
     </row>
@@ -1264,15 +1274,15 @@
         <v>44</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
-        <v>0.97999999999999987</v>
+        <f t="shared" si="2"/>
+        <v>3.6199999999999997</v>
       </c>
       <c r="D48">
-        <f>(A48^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>3.8719999999999999</v>
       </c>
     </row>
@@ -1281,15 +1291,15 @@
         <v>45</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
-        <v>0.99999999999999989</v>
+        <f t="shared" si="2"/>
+        <v>3.6999999999999997</v>
       </c>
       <c r="D49">
-        <f>(A49^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>4.05</v>
       </c>
     </row>
@@ -1298,15 +1308,15 @@
         <v>46</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
-        <v>1.02</v>
+        <f t="shared" si="2"/>
+        <v>3.78</v>
       </c>
       <c r="D50">
-        <f>(A50^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>4.2320000000000002</v>
       </c>
     </row>
@@ -1315,15 +1325,15 @@
         <v>47</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.4E-2</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
-        <v>1.04</v>
+        <f t="shared" si="2"/>
+        <v>3.86</v>
       </c>
       <c r="D51">
-        <f>(A51^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>4.4180000000000001</v>
       </c>
     </row>
@@ -1332,15 +1342,15 @@
         <v>48</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="C52">
-        <f t="shared" si="1"/>
-        <v>1.06</v>
+        <f t="shared" si="2"/>
+        <v>3.94</v>
       </c>
       <c r="D52">
-        <f>(A52^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>4.6080000000000005</v>
       </c>
     </row>
@@ -1349,15 +1359,15 @@
         <v>49</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="C53">
-        <f t="shared" si="1"/>
-        <v>1.08</v>
+        <f t="shared" si="2"/>
+        <v>4.0199999999999996</v>
       </c>
       <c r="D53">
-        <f>(A53^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>4.8020000000000005</v>
       </c>
     </row>
@@ -1366,15 +1376,15 @@
         <v>50</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="C54">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="2"/>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D54">
-        <f>(A54^2)*$R$1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>

</xml_diff>